<commit_message>
Water Data SA Download Code
</commit_message>
<xml_diff>
--- a/scripts/dataimport/hydro/WaterDataSA/Vars.xlsx
+++ b/scripts/dataimport/hydro/WaterDataSA/Vars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\GITHUB\CDM\scripts\dataimport\hydro\WaterDataSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\CDM\scripts\dataimport\hydro\WaterDataSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FDC679-BBED-4ADE-9CB9-81A3EC866F47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11B1A28-9109-4109-869D-798EB1B7888D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6150" yWindow="3800" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vars" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>AIRPRESSURE</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>WQ_OXY_OXY_SAT</t>
+  </si>
+  <si>
+    <t>isSonde</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>fDOM_SONDE</t>
+  </si>
+  <si>
+    <t>fDOM</t>
   </si>
 </sst>
 </file>
@@ -957,19 +969,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -977,10 +990,13 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -988,10 +1004,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -999,10 +1018,13 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1010,10 +1032,13 @@
         <v>15</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1021,21 +1046,28 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f>1000/86400</f>
+        <v>1.1574074074074073E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1043,10 +1075,13 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1054,10 +1089,13 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1065,10 +1103,13 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1076,10 +1117,13 @@
         <v>5</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1089,8 +1133,11 @@
       <c r="C11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1098,10 +1145,13 @@
         <v>7</v>
       </c>
       <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1109,10 +1159,13 @@
         <v>8</v>
       </c>
       <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1120,10 +1173,13 @@
         <v>9</v>
       </c>
       <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1131,10 +1187,13 @@
         <v>20</v>
       </c>
       <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1144,8 +1203,11 @@
       <c r="C16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1155,8 +1217,11 @@
       <c r="C17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1164,10 +1229,13 @@
         <v>18</v>
       </c>
       <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1177,8 +1245,11 @@
       <c r="C19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1188,8 +1259,11 @@
       <c r="C20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1199,8 +1273,12 @@
       <c r="C21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f>1000/32</f>
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1208,6 +1286,23 @@
         <v>13</v>
       </c>
       <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Water Data SA scripts
</commit_message>
<xml_diff>
--- a/scripts/dataimport/hydro/WaterDataSA/Vars.xlsx
+++ b/scripts/dataimport/hydro/WaterDataSA/Vars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\CDM\scripts\dataimport\hydro\WaterDataSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\scripts\dataimport\hydro\WaterDataSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11B1A28-9109-4109-869D-798EB1B7888D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9921C677-1230-4FD5-8C7C-83F11E378847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6150" yWindow="3800" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vars" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>AIRPRESSURE</t>
   </si>
@@ -129,6 +129,30 @@
   </si>
   <si>
     <t>fDOM</t>
+  </si>
+  <si>
+    <t>COND_BOTTOM</t>
+  </si>
+  <si>
+    <t>COND_SURFACE</t>
+  </si>
+  <si>
+    <t>CONDB</t>
+  </si>
+  <si>
+    <t>CONDS</t>
+  </si>
+  <si>
+    <t>TEMPS</t>
+  </si>
+  <si>
+    <t>TEMPB</t>
+  </si>
+  <si>
+    <t>TEMP_SURFACE</t>
+  </si>
+  <si>
+    <t>TEMP_BOTTOM</t>
   </si>
 </sst>
 </file>
@@ -969,20 +993,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -996,7 +1020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1024,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1038,7 +1062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1053,7 +1077,7 @@
         <v>1.1574074074074073E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1067,7 +1091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1081,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1095,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1109,7 +1133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1123,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1137,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1151,7 +1175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1165,7 +1189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1179,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1193,7 +1217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1207,7 +1231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1221,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1235,7 +1259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1249,7 +1273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1263,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1278,7 +1302,7 @@
         <v>31.25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1292,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1303,6 +1327,62 @@
         <v>1</v>
       </c>
       <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated WDSA data import and summary maps
</commit_message>
<xml_diff>
--- a/scripts/dataimport/hydro/WaterDataSA/Vars.xlsx
+++ b/scripts/dataimport/hydro/WaterDataSA/Vars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\scripts\dataimport\hydro\WaterDataSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9921C677-1230-4FD5-8C7C-83F11E378847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DA7719-32EE-4BE8-8EF7-D21297364A3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>AIRPRESSURE</t>
   </si>
@@ -74,9 +74,6 @@
     <t>WQ_PHY_BGA</t>
   </si>
   <si>
-    <t>WQ_DIAG_TOT_TCHLA</t>
-  </si>
-  <si>
     <t>COND</t>
   </si>
   <si>
@@ -153,6 +150,12 @@
   </si>
   <si>
     <t>TEMP_BOTTOM</t>
+  </si>
+  <si>
+    <t>isMet</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_PHY_TCHLA</t>
   </si>
 </sst>
 </file>
@@ -993,20 +996,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="3" max="4" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1014,13 +1017,16 @@
         <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1033,8 +1039,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1047,22 +1056,28 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1073,25 +1088,31 @@
         <v>0</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <f>1000/86400</f>
         <v>1.1574074074074073E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1104,8 +1125,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1118,8 +1142,11 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1130,10 +1157,13 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1144,12 +1174,15 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -1158,10 +1191,13 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1172,10 +1208,13 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1188,8 +1227,11 @@
       <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1202,109 +1244,133 @@
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
         <f>1000/32</f>
         <v>31.25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
         <v>13</v>
@@ -1313,76 +1379,94 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>32</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>33</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>35</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
         <v>36</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>39</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>37</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" t="s">
-        <v>38</v>
-      </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Water Data SA calculations using TDS for SAL.
</commit_message>
<xml_diff>
--- a/scripts/dataimport/hydro/WaterDataSA/Vars.xlsx
+++ b/scripts/dataimport/hydro/WaterDataSA/Vars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\scripts\dataimport\hydro\WaterDataSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DA7719-32EE-4BE8-8EF7-D21297364A3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9B18C8-ABF6-42BE-85E4-501E8FFAB2D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -999,7 +999,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,8 +1091,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <f>1000/86400</f>
-        <v>1.1574074074074073E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>